<commit_message>
first commit from maveenproject to github
</commit_message>
<xml_diff>
--- a/TextNgproject/textngart/assert.ng/excel.xlsx.xlsx
+++ b/TextNgproject/textngart/assert.ng/excel.xlsx.xlsx
@@ -14,15 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>qwswd</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>eerer</t>
   </si>
   <si>
     <t>wwww</t>
+  </si>
+  <si>
+    <t>harika</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>bava@123</t>
+  </si>
+  <si>
+    <t>anam</t>
   </si>
 </sst>
 </file>
@@ -46,15 +55,15 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -506,12 +515,12 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -636,8 +645,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -957,23 +968,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <cols>
+    <col min="8" max="8" width="10.6666666666667"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1">
+        <v>12345</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -986,7 +1000,32 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="3:8">
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="8:8">
+      <c r="H9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="8:8">
+      <c r="H10" s="1"/>
+    </row>
+    <row r="12" spans="6:6">
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H8" r:id="rId1" display="abc@gmail.com" tooltip="mailto:abc@gmail.com"/>
+    <hyperlink ref="H9" r:id="rId2" display="bava@123"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>